<commit_message>
Code for Figs 1,2,3
</commit_message>
<xml_diff>
--- a/Baleen-PFAS master sample list.xlsx
+++ b/Baleen-PFAS master sample list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavoca/Documents/Research Data/Whale research/Baleen project (PRFB : PFAS)/2020 (URI sampling)/Baleen_PFAS_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6562A9D0-8A4D-794F-8B30-742A148A121F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8431807D-E26F-4A42-9C86-97541D9BDDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F1E7AAD3-E57F-9640-B700-15A204BA8B7E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{F1E7AAD3-E57F-9640-B700-15A204BA8B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="204">
   <si>
     <t>Sample_num</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Adult</t>
   </si>
   <si>
-    <t>Calf/Yearling</t>
-  </si>
-  <si>
     <t>Yearling</t>
   </si>
   <si>
@@ -598,13 +595,70 @@
   </si>
   <si>
     <t>GLBW1-61-9</t>
+  </si>
+  <si>
+    <t>SciName</t>
+  </si>
+  <si>
+    <t>Megaptera novaeangliae</t>
+  </si>
+  <si>
+    <t>Eubalaena glacialis</t>
+  </si>
+  <si>
+    <t>Balaenoptera acutorostrata</t>
+  </si>
+  <si>
+    <t>Balaenoptera musculus</t>
+  </si>
+  <si>
+    <t>Balaenoptera physalus</t>
+  </si>
+  <si>
+    <t>Balaenoptera borealis</t>
+  </si>
+  <si>
+    <t>Free-swimming with gillnet gear. Found anchored on 12Sep2014. Gillnet panel lodged in mouth and tightly wrapping forward part of body. Panel entangled in pots with 20+ wraps of pot lines around flukes and peduncle. Mostly disentangled - left with short section of gillnet in mouth expecting to shed. Animal entangled again (14May2015 - anchored and disentangled). Carcass found 11Jun2015. Necropsy revealed gillnet from 2014 entanglement embedded deep into the maxilla and through the vomer. Bone had started to grow around the line. Gillnet is unknown origin. Pot/trap is US gear. </t>
+  </si>
+  <si>
+    <t>Fresh carcass with evidence of extensive constricting entanglement. No gear present. No necropsy, but robust body condition and histopathology results of samples support entanglement as COD. </t>
+  </si>
+  <si>
+    <t>Little Cranberry Island</t>
+  </si>
+  <si>
+    <t>Evidence of underwater entrapment and subsequent drowning. No gear present. </t>
+  </si>
+  <si>
+    <t>Fresh carcass with line impression across ventral surface and evidence of constricting gear around peduncle and fluke insertion. Bruising evident at fluke injuries. No gear present. </t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -648,6 +702,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -684,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -706,7 +774,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3132,8 +3201,8 @@
   <dimension ref="A1:J252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C215" sqref="C215"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E172" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3178,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3265,7 +3334,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3289,7 +3358,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6">
         <v>0.24229999999999999</v>
@@ -3614,7 +3683,7 @@
         <v>0.2641</v>
       </c>
       <c r="H20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -3637,7 +3706,7 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="H21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3660,7 +3729,7 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="H22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -3683,7 +3752,7 @@
         <v>0.25230000000000002</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -3706,7 +3775,7 @@
         <v>0.2465</v>
       </c>
       <c r="H24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -3729,7 +3798,7 @@
         <v>0.25380000000000003</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -3752,7 +3821,7 @@
         <v>0.25009999999999999</v>
       </c>
       <c r="H26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -3775,7 +3844,7 @@
         <v>0.25330000000000003</v>
       </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -3798,7 +3867,7 @@
         <v>0.26140000000000002</v>
       </c>
       <c r="H28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -3821,7 +3890,7 @@
         <v>0.25440000000000002</v>
       </c>
       <c r="H29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3844,7 +3913,7 @@
         <v>0.26019999999999999</v>
       </c>
       <c r="H30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3867,7 +3936,7 @@
         <v>0.26029999999999998</v>
       </c>
       <c r="H31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3890,7 +3959,7 @@
         <v>0.26850000000000002</v>
       </c>
       <c r="H32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3979,7 +4048,7 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -4002,7 +4071,7 @@
         <v>0.26119999999999999</v>
       </c>
       <c r="H37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -4025,7 +4094,7 @@
         <v>0.26340000000000002</v>
       </c>
       <c r="H38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -4048,10 +4117,10 @@
         <v>0.2482</v>
       </c>
       <c r="H39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -4074,10 +4143,10 @@
         <v>0.26219999999999999</v>
       </c>
       <c r="H40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -4100,10 +4169,10 @@
         <v>0.25540000000000002</v>
       </c>
       <c r="H41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -4126,10 +4195,10 @@
         <v>0.24440000000000001</v>
       </c>
       <c r="H42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -4152,10 +4221,10 @@
         <v>0.26350000000000001</v>
       </c>
       <c r="H43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -4178,10 +4247,10 @@
         <v>0.25330000000000003</v>
       </c>
       <c r="H44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -4204,10 +4273,10 @@
         <v>0.26790000000000003</v>
       </c>
       <c r="H45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -4230,7 +4299,7 @@
         <v>14</v>
       </c>
       <c r="I46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -4256,7 +4325,7 @@
         <v>26</v>
       </c>
       <c r="I47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -4282,7 +4351,7 @@
         <v>27</v>
       </c>
       <c r="I48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -4308,7 +4377,7 @@
         <v>20</v>
       </c>
       <c r="I49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4334,7 +4403,7 @@
         <v>22</v>
       </c>
       <c r="I50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -4357,10 +4426,10 @@
         <v>0.2656</v>
       </c>
       <c r="H51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -4383,10 +4452,10 @@
         <v>0.26669999999999999</v>
       </c>
       <c r="H52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -4409,10 +4478,10 @@
         <v>0.24940000000000001</v>
       </c>
       <c r="H53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -4435,10 +4504,10 @@
         <v>0.24940000000000001</v>
       </c>
       <c r="H54" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -4461,13 +4530,13 @@
         <v>0.26029999999999998</v>
       </c>
       <c r="H55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -4490,10 +4559,10 @@
         <v>0.2626</v>
       </c>
       <c r="H56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -4516,10 +4585,10 @@
         <v>0.25230000000000002</v>
       </c>
       <c r="H57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -4542,10 +4611,10 @@
         <v>0.24679999999999999</v>
       </c>
       <c r="H58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -4568,10 +4637,10 @@
         <v>0.25829999999999997</v>
       </c>
       <c r="H59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -4594,10 +4663,10 @@
         <v>0.26269999999999999</v>
       </c>
       <c r="H60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -4620,10 +4689,10 @@
         <v>0.26650000000000001</v>
       </c>
       <c r="H61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -4646,10 +4715,10 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="H62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -4672,10 +4741,10 @@
         <v>0.2472</v>
       </c>
       <c r="H63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -4698,10 +4767,10 @@
         <v>0.26040000000000002</v>
       </c>
       <c r="H64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -4724,10 +4793,10 @@
         <v>0.25559999999999999</v>
       </c>
       <c r="H65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -4750,10 +4819,10 @@
         <v>0.24160000000000001</v>
       </c>
       <c r="H66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -4776,10 +4845,10 @@
         <v>0.2472</v>
       </c>
       <c r="H67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -4802,10 +4871,10 @@
         <v>0.27629999999999999</v>
       </c>
       <c r="H68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -4828,7 +4897,7 @@
         <v>14</v>
       </c>
       <c r="I69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -4854,7 +4923,7 @@
         <v>20</v>
       </c>
       <c r="I70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -4880,7 +4949,7 @@
         <v>22</v>
       </c>
       <c r="I71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -4903,10 +4972,10 @@
         <v>0.24610000000000001</v>
       </c>
       <c r="H72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -4929,7 +4998,7 @@
         <v>14</v>
       </c>
       <c r="I73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -4955,7 +5024,7 @@
         <v>20</v>
       </c>
       <c r="I74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -4981,7 +5050,7 @@
         <v>22</v>
       </c>
       <c r="I75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -5004,7 +5073,7 @@
         <v>14</v>
       </c>
       <c r="I76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -5030,7 +5099,7 @@
         <v>20</v>
       </c>
       <c r="I77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -5056,7 +5125,7 @@
         <v>22</v>
       </c>
       <c r="I78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -5079,10 +5148,10 @@
         <v>0.27150000000000002</v>
       </c>
       <c r="H79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -5108,7 +5177,7 @@
         <v>22</v>
       </c>
       <c r="I80" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -5131,10 +5200,10 @@
         <v>0.26889999999999997</v>
       </c>
       <c r="H81" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -5157,10 +5226,10 @@
         <v>0.25569999999999998</v>
       </c>
       <c r="H82" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I82" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -5183,10 +5252,10 @@
         <v>0.25090000000000001</v>
       </c>
       <c r="H83" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I83" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -5209,10 +5278,10 @@
         <v>0.17929999999999999</v>
       </c>
       <c r="H84" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -5235,10 +5304,10 @@
         <v>0.26919999999999999</v>
       </c>
       <c r="H85" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -5261,10 +5330,10 @@
         <v>0.26469999999999999</v>
       </c>
       <c r="H86" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I86" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -5287,10 +5356,10 @@
         <v>0.18310000000000001</v>
       </c>
       <c r="H87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I87" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -5313,7 +5382,7 @@
         <v>0.24229999999999999</v>
       </c>
       <c r="H88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -5768,7 +5837,7 @@
         <v>0.25690000000000002</v>
       </c>
       <c r="H113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
@@ -5791,7 +5860,7 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="H114" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -5814,7 +5883,7 @@
         <v>0.26450000000000001</v>
       </c>
       <c r="H115" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -5837,7 +5906,7 @@
         <v>0.2681</v>
       </c>
       <c r="H116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -5860,7 +5929,7 @@
         <v>0.24310000000000001</v>
       </c>
       <c r="H117" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -5883,7 +5952,7 @@
         <v>0.24229999999999999</v>
       </c>
       <c r="H118" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -5906,7 +5975,7 @@
         <v>0.26769999999999999</v>
       </c>
       <c r="H119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
@@ -5929,7 +5998,7 @@
         <v>0.2646</v>
       </c>
       <c r="H120" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -5952,7 +6021,7 @@
         <v>0.25209999999999999</v>
       </c>
       <c r="H121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -5975,7 +6044,7 @@
         <v>0.245</v>
       </c>
       <c r="H122" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -5998,7 +6067,7 @@
         <v>0.2359</v>
       </c>
       <c r="H123" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -6021,7 +6090,7 @@
         <v>0.24060000000000001</v>
       </c>
       <c r="H124" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -6044,7 +6113,7 @@
         <v>0.25459999999999999</v>
       </c>
       <c r="H125" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -6067,7 +6136,7 @@
         <v>0.2359</v>
       </c>
       <c r="H126" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -6090,7 +6159,7 @@
         <v>0.2369</v>
       </c>
       <c r="H127" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I127" t="s">
         <v>49</v>
@@ -6116,7 +6185,7 @@
         <v>0.254</v>
       </c>
       <c r="H128" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -6139,7 +6208,7 @@
         <v>0.23519999999999999</v>
       </c>
       <c r="H129" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
@@ -6162,7 +6231,7 @@
         <v>0.253</v>
       </c>
       <c r="H130" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -6185,7 +6254,7 @@
         <v>0.26090000000000002</v>
       </c>
       <c r="H131" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -6208,7 +6277,7 @@
         <v>0.24340000000000001</v>
       </c>
       <c r="H132" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I132" t="s">
         <v>51</v>
@@ -6234,7 +6303,7 @@
         <v>0.24579999999999999</v>
       </c>
       <c r="H133" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -6257,7 +6326,7 @@
         <v>0.24329999999999999</v>
       </c>
       <c r="H134" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -6280,7 +6349,7 @@
         <v>0.25569999999999998</v>
       </c>
       <c r="H135" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I135" t="s">
         <v>49</v>
@@ -6361,7 +6430,7 @@
         <v>41</v>
       </c>
       <c r="H138" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -6387,7 +6456,7 @@
         <v>41</v>
       </c>
       <c r="H139" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -6413,7 +6482,7 @@
         <v>41</v>
       </c>
       <c r="H140" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -6439,7 +6508,7 @@
         <v>41</v>
       </c>
       <c r="H141" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6465,7 +6534,7 @@
         <v>41</v>
       </c>
       <c r="H142" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6491,7 +6560,7 @@
         <v>41</v>
       </c>
       <c r="H143" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6517,7 +6586,7 @@
         <v>41</v>
       </c>
       <c r="H144" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6543,7 +6612,7 @@
         <v>41</v>
       </c>
       <c r="H145" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I145" t="s">
         <v>49</v>
@@ -6572,7 +6641,7 @@
         <v>41</v>
       </c>
       <c r="H146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6598,7 +6667,7 @@
         <v>41</v>
       </c>
       <c r="H147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -6624,7 +6693,7 @@
         <v>41</v>
       </c>
       <c r="H148" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6650,7 +6719,7 @@
         <v>41</v>
       </c>
       <c r="H149" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -6676,7 +6745,7 @@
         <v>41</v>
       </c>
       <c r="H150" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -6702,7 +6771,7 @@
         <v>41</v>
       </c>
       <c r="H151" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -6728,7 +6797,7 @@
         <v>41</v>
       </c>
       <c r="H152" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -6754,7 +6823,7 @@
         <v>41</v>
       </c>
       <c r="H153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -6780,7 +6849,7 @@
         <v>41</v>
       </c>
       <c r="H154" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
@@ -6806,7 +6875,7 @@
         <v>41</v>
       </c>
       <c r="H155" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -6832,7 +6901,7 @@
         <v>41</v>
       </c>
       <c r="H156" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -6858,7 +6927,7 @@
         <v>41</v>
       </c>
       <c r="H157" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -6884,7 +6953,7 @@
         <v>41</v>
       </c>
       <c r="H158" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -6910,7 +6979,7 @@
         <v>41</v>
       </c>
       <c r="H159" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6936,7 +7005,7 @@
         <v>41</v>
       </c>
       <c r="H160" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
@@ -6962,7 +7031,7 @@
         <v>41</v>
       </c>
       <c r="H161" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
@@ -6988,7 +7057,7 @@
         <v>41</v>
       </c>
       <c r="H162" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
@@ -7014,7 +7083,7 @@
         <v>41</v>
       </c>
       <c r="H163" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
@@ -7040,7 +7109,7 @@
         <v>41</v>
       </c>
       <c r="H164" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -7066,7 +7135,7 @@
         <v>41</v>
       </c>
       <c r="H165" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I165" t="s">
         <v>50</v>
@@ -7095,7 +7164,7 @@
         <v>41</v>
       </c>
       <c r="H166" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I166" t="s">
         <v>50</v>
@@ -7124,7 +7193,7 @@
         <v>41</v>
       </c>
       <c r="H167" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I167" t="s">
         <v>50</v>
@@ -7153,127 +7222,130 @@
         <v>41</v>
       </c>
       <c r="H168" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I168" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="13">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A169">
         <v>168</v>
       </c>
-      <c r="B169" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C169" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D169" s="13" t="s">
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" t="s">
+        <v>17</v>
+      </c>
+      <c r="D169" t="s">
         <v>40</v>
       </c>
-      <c r="E169" s="13">
+      <c r="E169">
         <v>34</v>
       </c>
-      <c r="F169" s="13">
+      <c r="F169">
         <v>0.24060000000000001</v>
       </c>
-      <c r="G169" s="13" t="s">
+      <c r="G169" t="s">
         <v>41</v>
       </c>
-      <c r="H169" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="I169" s="13" t="s">
+      <c r="H169" t="s">
+        <v>183</v>
+      </c>
+      <c r="I169" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="170" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="13">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A170">
         <v>169</v>
       </c>
-      <c r="B170" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C170" s="13" t="s">
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" t="s">
         <v>42</v>
       </c>
-      <c r="D170" s="13" t="s">
+      <c r="D170" t="s">
         <v>43</v>
       </c>
-      <c r="F170" s="13">
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
         <v>0.253</v>
       </c>
-      <c r="H170" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="13">
+      <c r="H170" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A171">
         <v>170</v>
       </c>
-      <c r="B171" s="13" t="s">
+      <c r="B171" t="s">
         <v>14</v>
       </c>
-      <c r="C171" s="13" t="s">
+      <c r="C171" t="s">
         <v>42</v>
       </c>
-      <c r="D171" s="13" t="s">
+      <c r="D171" t="s">
         <v>44</v>
       </c>
-      <c r="F171" s="13">
+      <c r="F171">
         <v>0.27550000000000002</v>
       </c>
-      <c r="H171" s="13" t="s">
+      <c r="H171" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="13">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A172">
         <v>171</v>
       </c>
-      <c r="B172" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C172" s="13" t="s">
+      <c r="B172" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172" t="s">
         <v>42</v>
       </c>
-      <c r="D172" s="13" t="s">
+      <c r="D172" t="s">
         <v>44</v>
       </c>
-      <c r="E172" s="13">
+      <c r="E172">
         <v>1</v>
       </c>
-      <c r="F172" s="13">
+      <c r="F172">
         <v>0.23569999999999999</v>
       </c>
-      <c r="H172" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="13">
+      <c r="H172" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A173">
         <v>172</v>
       </c>
-      <c r="B173" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D173" s="13" t="s">
+      <c r="B173" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" t="s">
+        <v>17</v>
+      </c>
+      <c r="D173" t="s">
         <v>45</v>
       </c>
-      <c r="E173" s="13">
+      <c r="E173">
         <v>1</v>
       </c>
-      <c r="F173" s="13">
+      <c r="F173">
         <v>0.26229999999999998</v>
       </c>
-      <c r="G173" s="13" t="s">
+      <c r="G173" t="s">
         <v>46</v>
       </c>
-      <c r="H173" s="13" t="s">
+      <c r="H173" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7325,8 +7397,8 @@
       <c r="G175" t="s">
         <v>46</v>
       </c>
-      <c r="H175" s="13" t="s">
-        <v>153</v>
+      <c r="H175" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -7351,8 +7423,8 @@
       <c r="G176" t="s">
         <v>46</v>
       </c>
-      <c r="H176" s="13" t="s">
-        <v>154</v>
+      <c r="H176" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -7377,8 +7449,8 @@
       <c r="G177" t="s">
         <v>46</v>
       </c>
-      <c r="H177" s="13" t="s">
-        <v>155</v>
+      <c r="H177" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -7403,8 +7475,8 @@
       <c r="G178" t="s">
         <v>46</v>
       </c>
-      <c r="H178" s="13" t="s">
-        <v>156</v>
+      <c r="H178" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -7429,8 +7501,8 @@
       <c r="G179" t="s">
         <v>46</v>
       </c>
-      <c r="H179" s="13" t="s">
-        <v>157</v>
+      <c r="H179" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -7455,8 +7527,8 @@
       <c r="G180" t="s">
         <v>46</v>
       </c>
-      <c r="H180" s="13" t="s">
-        <v>158</v>
+      <c r="H180" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -7481,8 +7553,8 @@
       <c r="G181" t="s">
         <v>46</v>
       </c>
-      <c r="H181" s="13" t="s">
-        <v>159</v>
+      <c r="H181" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -7507,8 +7579,8 @@
       <c r="G182" t="s">
         <v>46</v>
       </c>
-      <c r="H182" s="13" t="s">
-        <v>160</v>
+      <c r="H182" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -7533,8 +7605,8 @@
       <c r="G183" t="s">
         <v>46</v>
       </c>
-      <c r="H183" s="13" t="s">
-        <v>161</v>
+      <c r="H183" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -7559,8 +7631,8 @@
       <c r="G184" t="s">
         <v>46</v>
       </c>
-      <c r="H184" s="13" t="s">
-        <v>162</v>
+      <c r="H184" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -7585,8 +7657,8 @@
       <c r="G185" t="s">
         <v>46</v>
       </c>
-      <c r="H185" s="13" t="s">
-        <v>163</v>
+      <c r="H185" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -7611,8 +7683,8 @@
       <c r="G186" t="s">
         <v>46</v>
       </c>
-      <c r="H186" s="13" t="s">
-        <v>164</v>
+      <c r="H186" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -7637,8 +7709,8 @@
       <c r="G187" t="s">
         <v>46</v>
       </c>
-      <c r="H187" s="13" t="s">
-        <v>165</v>
+      <c r="H187" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -7663,8 +7735,8 @@
       <c r="G188" t="s">
         <v>46</v>
       </c>
-      <c r="H188" s="13" t="s">
-        <v>166</v>
+      <c r="H188" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -7689,8 +7761,8 @@
       <c r="G189" t="s">
         <v>46</v>
       </c>
-      <c r="H189" s="13" t="s">
-        <v>167</v>
+      <c r="H189" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -7715,8 +7787,8 @@
       <c r="G190" t="s">
         <v>46</v>
       </c>
-      <c r="H190" s="13" t="s">
-        <v>168</v>
+      <c r="H190" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
@@ -7741,8 +7813,8 @@
       <c r="G191" t="s">
         <v>46</v>
       </c>
-      <c r="H191" s="13" t="s">
-        <v>169</v>
+      <c r="H191" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
@@ -7767,8 +7839,8 @@
       <c r="G192" t="s">
         <v>46</v>
       </c>
-      <c r="H192" s="13" t="s">
-        <v>170</v>
+      <c r="H192" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
@@ -7793,8 +7865,8 @@
       <c r="G193" t="s">
         <v>46</v>
       </c>
-      <c r="H193" s="13" t="s">
-        <v>171</v>
+      <c r="H193" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
@@ -7819,8 +7891,8 @@
       <c r="G194" t="s">
         <v>46</v>
       </c>
-      <c r="H194" s="13" t="s">
-        <v>172</v>
+      <c r="H194" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
@@ -7845,8 +7917,8 @@
       <c r="G195" t="s">
         <v>46</v>
       </c>
-      <c r="H195" s="13" t="s">
-        <v>173</v>
+      <c r="H195" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
@@ -7871,8 +7943,8 @@
       <c r="G196" t="s">
         <v>46</v>
       </c>
-      <c r="H196" s="13" t="s">
-        <v>174</v>
+      <c r="H196" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
@@ -7897,8 +7969,8 @@
       <c r="G197" t="s">
         <v>46</v>
       </c>
-      <c r="H197" s="13" t="s">
-        <v>175</v>
+      <c r="H197" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -7923,8 +7995,8 @@
       <c r="G198" t="s">
         <v>46</v>
       </c>
-      <c r="H198" s="13" t="s">
-        <v>176</v>
+      <c r="H198" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
@@ -7949,8 +8021,8 @@
       <c r="G199" t="s">
         <v>46</v>
       </c>
-      <c r="H199" s="13" t="s">
-        <v>177</v>
+      <c r="H199" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
@@ -7975,8 +8047,8 @@
       <c r="G200" t="s">
         <v>46</v>
       </c>
-      <c r="H200" s="13" t="s">
-        <v>178</v>
+      <c r="H200" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
@@ -8045,7 +8117,7 @@
         <v>0.22989999999999999</v>
       </c>
       <c r="H203" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -8068,7 +8140,7 @@
         <v>0.2326</v>
       </c>
       <c r="H204" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -8091,7 +8163,7 @@
         <v>0.22989999999999999</v>
       </c>
       <c r="H205" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
@@ -8114,7 +8186,7 @@
         <v>0.24529999999999999</v>
       </c>
       <c r="H206" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
@@ -8137,7 +8209,7 @@
         <v>0.25359999999999999</v>
       </c>
       <c r="H207" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
@@ -8160,7 +8232,7 @@
         <v>0.2442</v>
       </c>
       <c r="H208" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
@@ -8183,7 +8255,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="H209" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
@@ -8206,7 +8278,7 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="H210" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
@@ -8284,7 +8356,7 @@
         <v>47</v>
       </c>
       <c r="H213" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
@@ -8310,7 +8382,7 @@
         <v>47</v>
       </c>
       <c r="H214" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
@@ -8336,7 +8408,7 @@
         <v>47</v>
       </c>
       <c r="H215" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
@@ -8362,7 +8434,7 @@
         <v>47</v>
       </c>
       <c r="H216" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
@@ -8388,7 +8460,7 @@
         <v>47</v>
       </c>
       <c r="H217" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
@@ -8414,7 +8486,7 @@
         <v>47</v>
       </c>
       <c r="H218" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
@@ -8440,7 +8512,7 @@
         <v>47</v>
       </c>
       <c r="H219" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
@@ -8466,7 +8538,7 @@
         <v>47</v>
       </c>
       <c r="H220" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
@@ -8492,7 +8564,7 @@
         <v>47</v>
       </c>
       <c r="H221" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
@@ -8518,7 +8590,7 @@
         <v>47</v>
       </c>
       <c r="H222" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
@@ -8544,7 +8616,7 @@
         <v>47</v>
       </c>
       <c r="H223" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
@@ -8570,7 +8642,7 @@
         <v>47</v>
       </c>
       <c r="H224" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
@@ -8596,7 +8668,7 @@
         <v>47</v>
       </c>
       <c r="H225" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
@@ -8622,7 +8694,7 @@
         <v>47</v>
       </c>
       <c r="H226" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
@@ -8648,7 +8720,7 @@
         <v>47</v>
       </c>
       <c r="H227" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
@@ -8674,7 +8746,7 @@
         <v>47</v>
       </c>
       <c r="H228" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
@@ -8700,7 +8772,7 @@
         <v>47</v>
       </c>
       <c r="H229" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
@@ -8726,7 +8798,7 @@
         <v>47</v>
       </c>
       <c r="H230" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
@@ -8752,7 +8824,7 @@
         <v>47</v>
       </c>
       <c r="H231" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
@@ -8778,7 +8850,7 @@
         <v>47</v>
       </c>
       <c r="H232" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
@@ -8804,7 +8876,7 @@
         <v>47</v>
       </c>
       <c r="H233" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
@@ -8830,7 +8902,7 @@
         <v>47</v>
       </c>
       <c r="H234" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
@@ -8908,7 +8980,7 @@
         <v>48</v>
       </c>
       <c r="H237" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
@@ -8934,7 +9006,7 @@
         <v>48</v>
       </c>
       <c r="H238" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
@@ -8960,7 +9032,7 @@
         <v>48</v>
       </c>
       <c r="H239" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
@@ -8986,7 +9058,7 @@
         <v>48</v>
       </c>
       <c r="H240" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.2">
@@ -9012,7 +9084,7 @@
         <v>48</v>
       </c>
       <c r="H241" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.2">
@@ -9038,7 +9110,7 @@
         <v>48</v>
       </c>
       <c r="H242" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.2">
@@ -9064,7 +9136,7 @@
         <v>48</v>
       </c>
       <c r="H243" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.2">
@@ -9090,7 +9162,7 @@
         <v>48</v>
       </c>
       <c r="H244" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.2">
@@ -9116,10 +9188,10 @@
         <v>48</v>
       </c>
       <c r="H245" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I245" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.2">
@@ -9145,7 +9217,7 @@
         <v>48</v>
       </c>
       <c r="H246" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.2">
@@ -9171,7 +9243,7 @@
         <v>48</v>
       </c>
       <c r="H247" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.2">
@@ -9197,7 +9269,7 @@
         <v>48</v>
       </c>
       <c r="H248" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.2">
@@ -9223,7 +9295,7 @@
         <v>48</v>
       </c>
       <c r="H249" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.2">
@@ -9249,7 +9321,7 @@
         <v>46</v>
       </c>
       <c r="H250" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.2">
@@ -9275,7 +9347,7 @@
         <v>46</v>
       </c>
       <c r="H251" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.2">
@@ -9301,7 +9373,7 @@
         <v>46</v>
       </c>
       <c r="H252" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -9314,1001 +9386,1269 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7D98F2-EE84-2E47-99D9-081926297FFB}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="U1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="2">
         <v>849</v>
       </c>
-      <c r="H2" s="7">
+      <c r="I2" s="7">
         <v>41549</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="K2" s="2">
+        <v>-70.789970999999994</v>
+      </c>
+      <c r="L2" s="2">
+        <v>41.525478</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="2">
         <v>3</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>957.5</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="7">
         <v>42712</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="K3" s="2">
+        <v>-70.113669000000002</v>
+      </c>
+      <c r="L3" s="2">
+        <v>42.066305999999997</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" s="2">
         <v>3</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>843</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="7">
         <v>42907</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="K4" s="2">
+        <v>-69.989789999999999</v>
+      </c>
+      <c r="L4" s="2">
+        <v>41.552247999999999</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" s="2">
         <v>1</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="P4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>1010</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="7">
         <v>42944</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="K5" s="2">
+        <v>-69.875489000000002</v>
+      </c>
+      <c r="L5" s="2">
+        <v>41.792023</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" s="2">
         <v>3</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="P5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>1360</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I6" s="7">
         <v>43593</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="K6" s="2">
+        <v>-70.242650999999995</v>
+      </c>
+      <c r="L6" s="2">
+        <v>42.024754000000001</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" s="2">
         <v>3</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="P6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>815</v>
       </c>
-      <c r="H7" s="7">
+      <c r="I7" s="7">
         <v>43873</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="J7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-70.066749999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>41.927160999999998</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="U7" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>108</v>
-      </c>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="2">
         <v>815</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="7">
         <v>42839</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="K8" s="2">
+        <v>-70.356320999999994</v>
+      </c>
+      <c r="L8" s="2">
+        <v>41.809303999999997</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="2">
         <v>3</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="P8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="7">
         <v>42311</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9">
+        <v>-124.42923399999999</v>
+      </c>
+      <c r="L9">
+        <v>42.406331999999999</v>
+      </c>
+      <c r="M9" t="s">
+        <v>202</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q9" s="2" t="s">
+      <c r="T9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="7">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="7">
         <v>40870</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="2">
+        <v>-117.262478</v>
+      </c>
+      <c r="L10">
+        <v>32.700906000000003</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U10" t="s">
+        <v>115</v>
+      </c>
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="7">
+        <v>42416</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="K11" s="2">
+        <v>-121.474113</v>
+      </c>
+      <c r="L11" s="2">
+        <v>35.922258999999997</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>116</v>
-      </c>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="R11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U11" t="s">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="7">
-        <v>42416</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>118</v>
-      </c>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="V11" s="4"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>860</v>
       </c>
-      <c r="H12" s="7">
+      <c r="I12" s="7">
         <v>42625</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="J12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="2">
+        <v>-70.598482000000004</v>
+      </c>
+      <c r="L12" s="2">
+        <v>41.349513999999999</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="2">
+      <c r="O12" s="2">
         <v>3</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="V12" s="4"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>74</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>524.20000000000005</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
         <v>41837</v>
       </c>
-      <c r="I13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K13">
+        <v>-67.712108000000001</v>
+      </c>
+      <c r="L13">
+        <v>44.496848</v>
+      </c>
+      <c r="M13" t="s">
+        <v>199</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K13">
+      <c r="O13">
         <v>3</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="P13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U13" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>75</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1078.9000000000001</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>42166</v>
       </c>
-      <c r="I14" t="s">
-        <v>92</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14">
+        <v>-68.180785999999998</v>
+      </c>
+      <c r="L14">
+        <v>44.368814</v>
+      </c>
+      <c r="M14" t="s">
+        <v>199</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K14">
+      <c r="O14">
         <v>4</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="P14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U14" t="s">
+        <v>101</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>75</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>1237.48</v>
       </c>
-      <c r="H15" s="6">
+      <c r="I15" s="6">
         <v>42530</v>
       </c>
-      <c r="I15" t="s">
-        <v>93</v>
-      </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15">
+        <v>-67.569787000000005</v>
+      </c>
+      <c r="L15">
+        <v>44.460493999999997</v>
+      </c>
+      <c r="M15" t="s">
+        <v>199</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K15">
+      <c r="O15">
         <v>4</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="P15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q15" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>48</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>73</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1097</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="6">
         <v>37895</v>
       </c>
-      <c r="I16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16">
+        <v>-69.510165000000001</v>
+      </c>
+      <c r="L16">
+        <v>43.833767999999999</v>
+      </c>
+      <c r="M16" t="s">
+        <v>199</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K16">
+      <c r="O16">
         <v>3</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="P16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>1360</v>
       </c>
-      <c r="H17" s="6">
+      <c r="I17" s="6">
         <v>43589</v>
       </c>
-      <c r="I17" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" t="s">
+        <v>93</v>
+      </c>
+      <c r="K17">
+        <v>-70.470726999999997</v>
+      </c>
+      <c r="L17">
+        <v>41.776237999999999</v>
+      </c>
+      <c r="M17" t="s">
+        <v>200</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K17">
+      <c r="O17">
         <v>3</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="P17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q17" t="s">
         <v>109</v>
       </c>
-      <c r="M17" t="s">
-        <v>110</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s">
-        <v>150</v>
+      <c r="C18" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="D18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" t="s">
         <v>67</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>74</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>503</v>
       </c>
-      <c r="H18" s="6">
+      <c r="I18" s="6">
         <v>44047</v>
       </c>
-      <c r="I18" t="s">
-        <v>95</v>
-      </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18">
+        <v>-68.648456999999993</v>
+      </c>
+      <c r="L18">
+        <v>44.047147000000002</v>
+      </c>
+      <c r="M18" t="s">
+        <v>199</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K18">
+      <c r="O18">
         <v>3</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="P18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M18" t="s">
+      <c r="S18" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
-        <v>150</v>
+      <c r="C19" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>75</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>777</v>
       </c>
-      <c r="H19" s="6">
+      <c r="I19" s="6">
         <v>44051</v>
       </c>
-      <c r="I19" t="s">
-        <v>96</v>
-      </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K19">
+        <v>-67.837220000000002</v>
+      </c>
+      <c r="L19">
+        <v>44.514197000000003</v>
+      </c>
+      <c r="M19" t="s">
+        <v>199</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K19">
+      <c r="O19">
         <v>4</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="P19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="G20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20">
+        <v>1097</v>
+      </c>
+      <c r="I20" s="4">
+        <v>41998</v>
+      </c>
+      <c r="J20" t="s">
+        <v>194</v>
+      </c>
+      <c r="K20">
+        <v>-68.22842</v>
+      </c>
+      <c r="L20">
+        <v>44.254587000000001</v>
+      </c>
+      <c r="M20" t="s">
+        <v>199</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
+      <c r="O20" s="2"/>
+      <c r="P20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q20" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>110</v>
+      <c r="R20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -10339,30 +10679,30 @@
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="10">
         <v>3.5</v>
@@ -10380,10 +10720,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="10">
         <v>2.5</v>
@@ -10401,10 +10741,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="10">
         <v>4</v>
@@ -10422,10 +10762,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="10">
         <v>0.5</v>
@@ -10443,10 +10783,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="10">
         <v>1.5</v>
@@ -10464,10 +10804,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="10">
         <v>0.3</v>
@@ -10485,10 +10825,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -10507,7 +10847,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -10526,7 +10866,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -10545,15 +10885,15 @@
         <v>24</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="10">
         <v>26</v>
@@ -10564,7 +10904,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -10572,7 +10912,7 @@
         <v>0.5</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G12" s="10">
         <v>9</v>
@@ -10583,7 +10923,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -10602,7 +10942,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -10610,7 +10950,7 @@
         <v>0.06</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G14" s="10">
         <v>2</v>
@@ -10621,7 +10961,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -10629,7 +10969,7 @@
         <v>0.3</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G15" s="10">
         <v>29</v>
@@ -10648,7 +10988,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -10685,28 +11025,28 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -10768,7 +11108,7 @@
         <v>53</v>
       </c>
       <c r="I3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K3" t="e">
         <f t="shared" ref="K3:K31" si="0">AVERAGE(I3:J3)</f>
@@ -10828,10 +11168,10 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K5" t="e">
         <f t="shared" si="0"/>
@@ -10918,10 +11258,10 @@
         <v>8</v>
       </c>
       <c r="I8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K8" t="e">
         <f t="shared" si="0"/>
@@ -10951,10 +11291,10 @@
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K9" t="e">
         <f t="shared" si="0"/>
@@ -10984,10 +11324,10 @@
         <v>8</v>
       </c>
       <c r="I10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K10" t="e">
         <f t="shared" si="0"/>
@@ -11111,10 +11451,10 @@
         <v>8</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K14" t="e">
         <f t="shared" si="0"/>
@@ -11174,10 +11514,10 @@
         <v>8</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K16" t="e">
         <f t="shared" si="0"/>

</xml_diff>